<commit_message>
case 8: finish Data To Excel
</commit_message>
<xml_diff>
--- a/TestMakeTools/bin/Debug/test.xlsx
+++ b/TestMakeTools/bin/Debug/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6600" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,86 +42,6 @@
   </si>
   <si>
     <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>k</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>o</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>u</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,15 +367,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,68 +394,8 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -549,46 +409,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>